<commit_message>
Wine Quality: regression techniques + good features prediction
</commit_message>
<xml_diff>
--- a/Wine Quality/NN_test_set_prediction_8222_bad_features_with_correlation.xlsx
+++ b/Wine Quality/NN_test_set_prediction_8222_bad_features_with_correlation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\Data Science\Deconstructing Neural Networks\Wine Quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{401C06A0-F06E-4B67-AAF2-68F47C6BD856}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF011020-E7F4-49B0-A54F-ABC6986C15BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="180" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-25320" yWindow="180" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NN_test_set_prediction_8222_bad" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NN_test_set_prediction_8222_bad!$A$1:$Q$107</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -166,7 +176,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -1036,11 +1046,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,7 +1059,8 @@
     <col min="1" max="1" width="36.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="13" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="14" max="17" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
@@ -1145,19 +1157,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N2" s="2">
-        <f>SUM(J2:M2)</f>
+        <f t="shared" ref="N2:N33" si="0">SUM(J2:M2)</f>
         <v>0.98519454069249357</v>
       </c>
       <c r="O2" s="2">
-        <f>ABS(J2)+ABS(K2)+ABS(L2)+ABS(M2)</f>
+        <f t="shared" ref="O2:O33" si="1">ABS(J2)+ABS(K2)+ABS(L2)+ABS(M2)</f>
         <v>0.98519454069249357</v>
       </c>
       <c r="P2" s="2">
-        <f>MIN(E2:I2)</f>
+        <f t="shared" ref="P2:P33" si="2">MIN(E2:I2)</f>
         <v>0.595117688179016</v>
       </c>
       <c r="Q2" s="2">
-        <f>AVERAGE(E2:I2)</f>
+        <f t="shared" ref="Q2:Q33" si="3">AVERAGE(E2:I2)</f>
         <v>0.61257967948913539</v>
       </c>
     </row>
@@ -1202,19 +1214,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N3" s="2">
-        <f>SUM(J3:M3)</f>
+        <f t="shared" si="0"/>
         <v>-1.0926312587260602E-2</v>
       </c>
       <c r="O3" s="2">
-        <f>ABS(J3)+ABS(K3)+ABS(L3)+ABS(M3)</f>
+        <f t="shared" si="1"/>
         <v>0.82671433548884132</v>
       </c>
       <c r="P3" s="2">
-        <f>MIN(E3:I3)</f>
+        <f t="shared" si="2"/>
         <v>0.59701687097549405</v>
       </c>
       <c r="Q3" s="2">
-        <f>AVERAGE(E3:I3)</f>
+        <f t="shared" si="3"/>
         <v>0.61512296199798566</v>
       </c>
     </row>
@@ -1259,19 +1271,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N4" s="2">
-        <f>SUM(J4:M4)</f>
+        <f t="shared" si="0"/>
         <v>-0.26952203611295761</v>
       </c>
       <c r="O4" s="2">
-        <f>ABS(J4)+ABS(K4)+ABS(L4)+ABS(M4)</f>
+        <f t="shared" si="1"/>
         <v>1.0964343530241005</v>
       </c>
       <c r="P4" s="2">
-        <f>MIN(E4:I4)</f>
+        <f t="shared" si="2"/>
         <v>0.59897661209106401</v>
       </c>
       <c r="Q4" s="2">
-        <f>AVERAGE(E4:I4)</f>
+        <f t="shared" si="3"/>
         <v>0.61551518440246533</v>
       </c>
     </row>
@@ -1316,19 +1328,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N5" s="2">
-        <f>SUM(J5:M5)</f>
+        <f t="shared" si="0"/>
         <v>0.38498986799297746</v>
       </c>
       <c r="O5" s="2">
-        <f>ABS(J5)+ABS(K5)+ABS(L5)+ABS(M5)</f>
+        <f t="shared" si="1"/>
         <v>1.0369983887240413</v>
       </c>
       <c r="P5" s="2">
-        <f>MIN(E5:I5)</f>
+        <f t="shared" si="2"/>
         <v>0.60186260938644398</v>
       </c>
       <c r="Q5" s="2">
-        <f>AVERAGE(E5:I5)</f>
+        <f t="shared" si="3"/>
         <v>0.61888102293014502</v>
       </c>
     </row>
@@ -1373,19 +1385,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N6" s="2">
-        <f>SUM(J6:M6)</f>
+        <f t="shared" si="0"/>
         <v>-0.45211917472328661</v>
       </c>
       <c r="O6" s="2">
-        <f>ABS(J6)+ABS(K6)+ABS(L6)+ABS(M6)</f>
+        <f t="shared" si="1"/>
         <v>0.93927750048538738</v>
       </c>
       <c r="P6" s="2">
-        <f>MIN(E6:I6)</f>
+        <f t="shared" si="2"/>
         <v>0.60404789447784402</v>
       </c>
       <c r="Q6" s="2">
-        <f>AVERAGE(E6:I6)</f>
+        <f t="shared" si="3"/>
         <v>0.61894611120223963</v>
       </c>
     </row>
@@ -1430,19 +1442,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N7" s="2">
-        <f>SUM(J7:M7)</f>
+        <f t="shared" si="0"/>
         <v>0.57197669627703751</v>
       </c>
       <c r="O7" s="2">
-        <f>ABS(J7)+ABS(K7)+ABS(L7)+ABS(M7)</f>
+        <f t="shared" si="1"/>
         <v>0.57197669627703751</v>
       </c>
       <c r="P7" s="2">
-        <f>MIN(E7:I7)</f>
+        <f t="shared" si="2"/>
         <v>0.60652095079421997</v>
       </c>
       <c r="Q7" s="2">
-        <f>AVERAGE(E7:I7)</f>
+        <f t="shared" si="3"/>
         <v>0.62085922956466644</v>
       </c>
     </row>
@@ -1487,19 +1499,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N8" s="2">
-        <f>SUM(J8:M8)</f>
+        <f t="shared" si="0"/>
         <v>-0.26602544141649148</v>
       </c>
       <c r="O8" s="2">
-        <f>ABS(J8)+ABS(K8)+ABS(L8)+ABS(M8)</f>
+        <f t="shared" si="1"/>
         <v>0.53932948653817836</v>
       </c>
       <c r="P8" s="2">
-        <f>MIN(E8:I8)</f>
+        <f t="shared" si="2"/>
         <v>0.60167771577835005</v>
       </c>
       <c r="Q8" s="2">
-        <f>AVERAGE(E8:I8)</f>
+        <f t="shared" si="3"/>
         <v>0.62259368896484324</v>
       </c>
     </row>
@@ -1544,19 +1556,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N9" s="2">
-        <f>SUM(J9:M9)</f>
+        <f t="shared" si="0"/>
         <v>-0.50037716087978357</v>
       </c>
       <c r="O9" s="2">
-        <f>ABS(J9)+ABS(K9)+ABS(L9)+ABS(M9)</f>
+        <f t="shared" si="1"/>
         <v>0.9875354866418844</v>
       </c>
       <c r="P9" s="2">
-        <f>MIN(E9:I9)</f>
+        <f t="shared" si="2"/>
         <v>0.60304224491119296</v>
       </c>
       <c r="Q9" s="2">
-        <f>AVERAGE(E9:I9)</f>
+        <f t="shared" si="3"/>
         <v>0.62297056913375803</v>
       </c>
     </row>
@@ -1601,19 +1613,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N10" s="2">
-        <f>SUM(J10:M10)</f>
+        <f t="shared" si="0"/>
         <v>-8.935522321539259E-2</v>
       </c>
       <c r="O10" s="2">
-        <f>ABS(J10)+ABS(K10)+ABS(L10)+ABS(M10)</f>
+        <f t="shared" si="1"/>
         <v>0.34783164372032577</v>
       </c>
       <c r="P10" s="2">
-        <f>MIN(E10:I10)</f>
+        <f t="shared" si="2"/>
         <v>0.60761725902557295</v>
       </c>
       <c r="Q10" s="2">
-        <f>AVERAGE(E10:I10)</f>
+        <f t="shared" si="3"/>
         <v>0.62555369138717598</v>
       </c>
     </row>
@@ -1658,19 +1670,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N11" s="2">
-        <f>SUM(J11:M11)</f>
+        <f t="shared" si="0"/>
         <v>-0.39515527215302698</v>
       </c>
       <c r="O11" s="2">
-        <f>ABS(J11)+ABS(K11)+ABS(L11)+ABS(M11)</f>
+        <f t="shared" si="1"/>
         <v>0.97080111698403115</v>
       </c>
       <c r="P11" s="2">
-        <f>MIN(E11:I11)</f>
+        <f t="shared" si="2"/>
         <v>0.61522835493087702</v>
       </c>
       <c r="Q11" s="2">
-        <f>AVERAGE(E11:I11)</f>
+        <f t="shared" si="3"/>
         <v>0.62585513591766317</v>
       </c>
     </row>
@@ -1715,19 +1727,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N12" s="2">
-        <f>SUM(J12:M12)</f>
+        <f t="shared" si="0"/>
         <v>0.42767830866692619</v>
       </c>
       <c r="O12" s="2">
-        <f>ABS(J12)+ABS(K12)+ABS(L12)+ABS(M12)</f>
+        <f t="shared" si="1"/>
         <v>1.0016222333403586</v>
       </c>
       <c r="P12" s="2">
-        <f>MIN(E12:I12)</f>
+        <f t="shared" si="2"/>
         <v>0.601615309715271</v>
       </c>
       <c r="Q12" s="2">
-        <f>AVERAGE(E12:I12)</f>
+        <f t="shared" si="3"/>
         <v>0.62703160047531104</v>
       </c>
     </row>
@@ -1772,19 +1784,19 @@
         <v>4.7400468259075297E-2</v>
       </c>
       <c r="N13" s="2">
-        <f>SUM(J13:M13)</f>
+        <f t="shared" si="0"/>
         <v>-0.1722713317861066</v>
       </c>
       <c r="O13" s="2">
-        <f>ABS(J13)+ABS(K13)+ABS(L13)+ABS(M13)</f>
+        <f t="shared" si="1"/>
         <v>0.63308359616856313</v>
       </c>
       <c r="P13" s="2">
-        <f>MIN(E13:I13)</f>
+        <f t="shared" si="2"/>
         <v>0.616277515888214</v>
       </c>
       <c r="Q13" s="2">
-        <f>AVERAGE(E13:I13)</f>
+        <f t="shared" si="3"/>
         <v>0.6275651693344112</v>
       </c>
     </row>
@@ -1829,19 +1841,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N14" s="2">
-        <f>SUM(J14:M14)</f>
+        <f t="shared" si="0"/>
         <v>-0.45815427566343786</v>
       </c>
       <c r="O14" s="2">
-        <f>ABS(J14)+ABS(K14)+ABS(L14)+ABS(M14)</f>
+        <f t="shared" si="1"/>
         <v>0.95169377580059877</v>
       </c>
       <c r="P14" s="2">
-        <f>MIN(E14:I14)</f>
+        <f t="shared" si="2"/>
         <v>0.61211109161376898</v>
       </c>
       <c r="Q14" s="2">
-        <f>AVERAGE(E14:I14)</f>
+        <f t="shared" si="3"/>
         <v>0.62789759635925235</v>
       </c>
     </row>
@@ -1886,19 +1898,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N15" s="2">
-        <f>SUM(J15:M15)</f>
+        <f t="shared" si="0"/>
         <v>-0.29813052051542971</v>
       </c>
       <c r="O15" s="2">
-        <f>ABS(J15)+ABS(K15)+ABS(L15)+ABS(M15)</f>
+        <f t="shared" si="1"/>
         <v>1.1117175309486069</v>
       </c>
       <c r="P15" s="2">
-        <f>MIN(E15:I15)</f>
+        <f t="shared" si="2"/>
         <v>0.60719311237335205</v>
       </c>
       <c r="Q15" s="2">
-        <f>AVERAGE(E15:I15)</f>
+        <f t="shared" si="3"/>
         <v>0.63002983331680262</v>
       </c>
     </row>
@@ -1943,19 +1955,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N16" s="2">
-        <f>SUM(J16:M16)</f>
+        <f t="shared" si="0"/>
         <v>0.49021175671973405</v>
       </c>
       <c r="O16" s="2">
-        <f>ABS(J16)+ABS(K16)+ABS(L16)+ABS(M16)</f>
+        <f t="shared" si="1"/>
         <v>1.020264019066188</v>
       </c>
       <c r="P16" s="2">
-        <f>MIN(E16:I16)</f>
+        <f t="shared" si="2"/>
         <v>0.62795174121856601</v>
       </c>
       <c r="Q16" s="2">
-        <f>AVERAGE(E16:I16)</f>
+        <f t="shared" si="3"/>
         <v>0.63015700578689537</v>
       </c>
     </row>
@@ -2000,19 +2012,19 @@
         <v>0.20063232664151201</v>
       </c>
       <c r="N17" s="2">
-        <f>SUM(J17:M17)</f>
+        <f t="shared" si="0"/>
         <v>0.2561653023685041</v>
       </c>
       <c r="O17" s="2">
-        <f>ABS(J17)+ABS(K17)+ABS(L17)+ABS(M17)</f>
+        <f t="shared" si="1"/>
         <v>0.51111067877882588</v>
       </c>
       <c r="P17" s="2">
-        <f>MIN(E17:I17)</f>
+        <f t="shared" si="2"/>
         <v>0.60595905780792203</v>
       </c>
       <c r="Q17" s="2">
-        <f>AVERAGE(E17:I17)</f>
+        <f t="shared" si="3"/>
         <v>0.63122036457061736</v>
       </c>
     </row>
@@ -2057,19 +2069,19 @@
         <v>0</v>
       </c>
       <c r="N18" s="2">
-        <f>SUM(J18:M18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O18" s="2">
-        <f>ABS(J18)+ABS(K18)+ABS(L18)+ABS(M18)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P18" s="2">
-        <f>MIN(E18:I18)</f>
+        <f t="shared" si="2"/>
         <v>0.59860438108444203</v>
       </c>
       <c r="Q18" s="2">
-        <f>AVERAGE(E18:I18)</f>
+        <f t="shared" si="3"/>
         <v>0.63239114284515363</v>
       </c>
     </row>
@@ -2114,19 +2126,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N19" s="2">
-        <f>SUM(J19:M19)</f>
+        <f t="shared" si="0"/>
         <v>0.17465213062377746</v>
       </c>
       <c r="O19" s="2">
-        <f>ABS(J19)+ABS(K19)+ABS(L19)+ABS(M19)</f>
+        <f t="shared" si="1"/>
         <v>1.2584604201028033</v>
       </c>
       <c r="P19" s="2">
-        <f>MIN(E19:I19)</f>
+        <f t="shared" si="2"/>
         <v>0.62648135423660201</v>
       </c>
       <c r="Q19" s="2">
-        <f>AVERAGE(E19:I19)</f>
+        <f t="shared" si="3"/>
         <v>0.63305253982543896</v>
       </c>
     </row>
@@ -2171,19 +2183,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N20" s="2">
-        <f>SUM(J20:M20)</f>
+        <f t="shared" si="0"/>
         <v>0.44381537436252949</v>
       </c>
       <c r="O20" s="2">
-        <f>ABS(J20)+ABS(K20)+ABS(L20)+ABS(M20)</f>
+        <f t="shared" si="1"/>
         <v>0.5768044923882415</v>
       </c>
       <c r="P20" s="2">
-        <f>MIN(E20:I20)</f>
+        <f t="shared" si="2"/>
         <v>0.61077451705932595</v>
       </c>
       <c r="Q20" s="2">
-        <f>AVERAGE(E20:I20)</f>
+        <f t="shared" si="3"/>
         <v>0.63399466276168781</v>
       </c>
     </row>
@@ -2228,19 +2240,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N21" s="2">
-        <f>SUM(J21:M21)</f>
+        <f t="shared" si="0"/>
         <v>0.98566009615009653</v>
       </c>
       <c r="O21" s="2">
-        <f>ABS(J21)+ABS(K21)+ABS(L21)+ABS(M21)</f>
+        <f t="shared" si="1"/>
         <v>0.98566009615009653</v>
       </c>
       <c r="P21" s="2">
-        <f>MIN(E21:I21)</f>
+        <f t="shared" si="2"/>
         <v>0.61397540569305398</v>
       </c>
       <c r="Q21" s="2">
-        <f>AVERAGE(E21:I21)</f>
+        <f t="shared" si="3"/>
         <v>0.63411220312118477</v>
       </c>
     </row>
@@ -2285,19 +2297,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N22" s="2">
-        <f>SUM(J22:M22)</f>
+        <f t="shared" si="0"/>
         <v>-0.1608035526897349</v>
       </c>
       <c r="O22" s="2">
-        <f>ABS(J22)+ABS(K22)+ABS(L22)+ABS(M22)</f>
+        <f t="shared" si="1"/>
         <v>0.52259511688032512</v>
       </c>
       <c r="P22" s="2">
-        <f>MIN(E22:I22)</f>
+        <f t="shared" si="2"/>
         <v>0.61334007978439298</v>
       </c>
       <c r="Q22" s="2">
-        <f>AVERAGE(E22:I22)</f>
+        <f t="shared" si="3"/>
         <v>0.63411660194396935</v>
       </c>
     </row>
@@ -2342,19 +2354,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N23" s="2">
-        <f>SUM(J23:M23)</f>
+        <f t="shared" si="0"/>
         <v>-0.24872377758127359</v>
       </c>
       <c r="O23" s="2">
-        <f>ABS(J23)+ABS(K23)+ABS(L23)+ABS(M23)</f>
+        <f t="shared" si="1"/>
         <v>0.74226327771843437</v>
       </c>
       <c r="P23" s="2">
-        <f>MIN(E23:I23)</f>
+        <f t="shared" si="2"/>
         <v>0.62656533718109098</v>
       </c>
       <c r="Q23" s="2">
-        <f>AVERAGE(E23:I23)</f>
+        <f t="shared" si="3"/>
         <v>0.63577172756195011</v>
       </c>
     </row>
@@ -2399,19 +2411,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N24" s="2">
-        <f>SUM(J24:M24)</f>
+        <f t="shared" si="0"/>
         <v>-0.42719795334215888</v>
       </c>
       <c r="O24" s="2">
-        <f>ABS(J24)+ABS(K24)+ABS(L24)+ABS(M24)</f>
+        <f t="shared" si="1"/>
         <v>0.70050199846384564</v>
       </c>
       <c r="P24" s="2">
-        <f>MIN(E24:I24)</f>
+        <f t="shared" si="2"/>
         <v>0.61154258251190097</v>
       </c>
       <c r="Q24" s="2">
-        <f>AVERAGE(E24:I24)</f>
+        <f t="shared" si="3"/>
         <v>0.63604180812835642</v>
       </c>
     </row>
@@ -2456,19 +2468,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N25" s="2">
-        <f>SUM(J25:M25)</f>
+        <f t="shared" si="0"/>
         <v>-0.21897297925537329</v>
       </c>
       <c r="O25" s="2">
-        <f>ABS(J25)+ABS(K25)+ABS(L25)+ABS(M25)</f>
+        <f t="shared" si="1"/>
         <v>1.1469834098816847</v>
       </c>
       <c r="P25" s="2">
-        <f>MIN(E25:I25)</f>
+        <f t="shared" si="2"/>
         <v>0.61532485485076904</v>
       </c>
       <c r="Q25" s="2">
-        <f>AVERAGE(E25:I25)</f>
+        <f t="shared" si="3"/>
         <v>0.63617295026779141</v>
       </c>
     </row>
@@ -2513,19 +2525,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N26" s="2">
-        <f>SUM(J26:M26)</f>
+        <f t="shared" si="0"/>
         <v>0.31803483999937676</v>
       </c>
       <c r="O26" s="2">
-        <f>ABS(J26)+ABS(K26)+ABS(L26)+ABS(M26)</f>
+        <f t="shared" si="1"/>
         <v>0.49491562035206715</v>
       </c>
       <c r="P26" s="2">
-        <f>MIN(E26:I26)</f>
+        <f t="shared" si="2"/>
         <v>0.62357795238494795</v>
       </c>
       <c r="Q26" s="2">
-        <f>AVERAGE(E26:I26)</f>
+        <f t="shared" si="3"/>
         <v>0.63645931482315021</v>
       </c>
     </row>
@@ -2570,19 +2582,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N27" s="2">
-        <f>SUM(J27:M27)</f>
+        <f t="shared" si="0"/>
         <v>-0.29067929169022688</v>
       </c>
       <c r="O27" s="2">
-        <f>ABS(J27)+ABS(K27)+ABS(L27)+ABS(M27)</f>
+        <f t="shared" si="1"/>
         <v>0.58769211513179687</v>
       </c>
       <c r="P27" s="2">
-        <f>MIN(E27:I27)</f>
+        <f t="shared" si="2"/>
         <v>0.63186037540435702</v>
       </c>
       <c r="Q27" s="2">
-        <f>AVERAGE(E27:I27)</f>
+        <f t="shared" si="3"/>
         <v>0.6378537893295283</v>
       </c>
     </row>
@@ -2627,19 +2639,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N28" s="2">
-        <f>SUM(J28:M28)</f>
+        <f t="shared" si="0"/>
         <v>-0.29337652750622778</v>
       </c>
       <c r="O28" s="2">
-        <f>ABS(J28)+ABS(K28)+ABS(L28)+ABS(M28)</f>
+        <f t="shared" si="1"/>
         <v>1.0725798616308304</v>
       </c>
       <c r="P28" s="2">
-        <f>MIN(E28:I28)</f>
+        <f t="shared" si="2"/>
         <v>0.62424463033676103</v>
       </c>
       <c r="Q28" s="2">
-        <f>AVERAGE(E28:I28)</f>
+        <f t="shared" si="3"/>
         <v>0.63857097625732384</v>
       </c>
     </row>
@@ -2684,19 +2696,19 @@
         <v>0.37126048128542699</v>
       </c>
       <c r="N29" s="2">
-        <f>SUM(J29:M29)</f>
+        <f t="shared" si="0"/>
         <v>0.95452352587318579</v>
       </c>
       <c r="O29" s="2">
-        <f>ABS(J29)+ABS(K29)+ABS(L29)+ABS(M29)</f>
+        <f t="shared" si="1"/>
         <v>1.1314043062258761</v>
       </c>
       <c r="P29" s="2">
-        <f>MIN(E29:I29)</f>
+        <f t="shared" si="2"/>
         <v>0.630487620830535</v>
       </c>
       <c r="Q29" s="2">
-        <f>AVERAGE(E29:I29)</f>
+        <f t="shared" si="3"/>
         <v>0.63858858346939018</v>
       </c>
     </row>
@@ -2741,19 +2753,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N30" s="2">
-        <f>SUM(J30:M30)</f>
+        <f t="shared" si="0"/>
         <v>0.34812212047819369</v>
       </c>
       <c r="O30" s="2">
-        <f>ABS(J30)+ABS(K30)+ABS(L30)+ABS(M30)</f>
+        <f t="shared" si="1"/>
         <v>0.34812212047819369</v>
       </c>
       <c r="P30" s="2">
-        <f>MIN(E30:I30)</f>
+        <f t="shared" si="2"/>
         <v>0.62818688154220503</v>
       </c>
       <c r="Q30" s="2">
-        <f>AVERAGE(E30:I30)</f>
+        <f t="shared" si="3"/>
         <v>0.639572417736053</v>
       </c>
     </row>
@@ -2798,19 +2810,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N31" s="2">
-        <f>SUM(J31:M31)</f>
+        <f t="shared" si="0"/>
         <v>-0.11759849991693426</v>
       </c>
       <c r="O31" s="2">
-        <f>ABS(J31)+ABS(K31)+ABS(L31)+ABS(M31)</f>
+        <f t="shared" si="1"/>
         <v>0.56580016965312574</v>
       </c>
       <c r="P31" s="2">
-        <f>MIN(E31:I31)</f>
+        <f t="shared" si="2"/>
         <v>0.61770433187484697</v>
       </c>
       <c r="Q31" s="2">
-        <f>AVERAGE(E31:I31)</f>
+        <f t="shared" si="3"/>
         <v>0.6396270513534541</v>
       </c>
     </row>
@@ -2855,19 +2867,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N32" s="2">
-        <f>SUM(J32:M32)</f>
+        <f t="shared" si="0"/>
         <v>-0.35622823269355536</v>
       </c>
       <c r="O32" s="2">
-        <f>ABS(J32)+ABS(K32)+ABS(L32)+ABS(M32)</f>
+        <f t="shared" si="1"/>
         <v>1.0097281564435028</v>
       </c>
       <c r="P32" s="2">
-        <f>MIN(E32:I32)</f>
+        <f t="shared" si="2"/>
         <v>0.61593687534332198</v>
       </c>
       <c r="Q32" s="2">
-        <f>AVERAGE(E32:I32)</f>
+        <f t="shared" si="3"/>
         <v>0.63964098691940252</v>
       </c>
     </row>
@@ -2912,19 +2924,19 @@
         <v>0.203822913829042</v>
       </c>
       <c r="N33" s="2">
-        <f>SUM(J33:M33)</f>
+        <f t="shared" si="0"/>
         <v>-0.19940029215863952</v>
       </c>
       <c r="O33" s="2">
-        <f>ABS(J33)+ABS(K33)+ABS(L33)+ABS(M33)</f>
+        <f t="shared" si="1"/>
         <v>0.71036126350238038</v>
       </c>
       <c r="P33" s="2">
-        <f>MIN(E33:I33)</f>
+        <f t="shared" si="2"/>
         <v>0.62430620193481401</v>
       </c>
       <c r="Q33" s="2">
-        <f>AVERAGE(E33:I33)</f>
+        <f t="shared" si="3"/>
         <v>0.63991533517837507</v>
       </c>
     </row>
@@ -2969,19 +2981,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N34" s="2">
-        <f>SUM(J34:M34)</f>
+        <f t="shared" ref="N34:N65" si="4">SUM(J34:M34)</f>
         <v>-0.30142636627230379</v>
       </c>
       <c r="O34" s="2">
-        <f>ABS(J34)+ABS(K34)+ABS(L34)+ABS(M34)</f>
+        <f t="shared" ref="O34:O65" si="5">ABS(J34)+ABS(K34)+ABS(L34)+ABS(M34)</f>
         <v>1.1864862812493642</v>
       </c>
       <c r="P34" s="2">
-        <f>MIN(E34:I34)</f>
+        <f t="shared" ref="P34:P65" si="6">MIN(E34:I34)</f>
         <v>0.62291187047958296</v>
       </c>
       <c r="Q34" s="2">
-        <f>AVERAGE(E34:I34)</f>
+        <f t="shared" ref="Q34:Q65" si="7">AVERAGE(E34:I34)</f>
         <v>0.64028881788253744</v>
       </c>
     </row>
@@ -3026,19 +3038,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N35" s="2">
-        <f>SUM(J35:M35)</f>
+        <f t="shared" si="4"/>
         <v>0.51249486075054373</v>
       </c>
       <c r="O35" s="2">
-        <f>ABS(J35)+ABS(K35)+ABS(L35)+ABS(M35)</f>
+        <f t="shared" si="5"/>
         <v>0.90579006535928375</v>
       </c>
       <c r="P35" s="2">
-        <f>MIN(E35:I35)</f>
+        <f t="shared" si="6"/>
         <v>0.61755800247192305</v>
       </c>
       <c r="Q35" s="2">
-        <f>AVERAGE(E35:I35)</f>
+        <f t="shared" si="7"/>
         <v>0.64087024927139224</v>
       </c>
     </row>
@@ -3083,19 +3095,19 @@
         <v>4.7400468259075297E-2</v>
       </c>
       <c r="N36" s="2">
-        <f>SUM(J36:M36)</f>
+        <f t="shared" si="4"/>
         <v>-0.33344384371177394</v>
       </c>
       <c r="O36" s="2">
-        <f>ABS(J36)+ABS(K36)+ABS(L36)+ABS(M36)</f>
+        <f t="shared" si="5"/>
         <v>0.79425610809423053</v>
       </c>
       <c r="P36" s="2">
-        <f>MIN(E36:I36)</f>
+        <f t="shared" si="6"/>
         <v>0.61883985996246305</v>
       </c>
       <c r="Q36" s="2">
-        <f>AVERAGE(E36:I36)</f>
+        <f t="shared" si="7"/>
         <v>0.64128450155258121</v>
       </c>
     </row>
@@ -3140,19 +3152,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N37" s="2">
-        <f>SUM(J37:M37)</f>
+        <f t="shared" si="4"/>
         <v>-0.54804944378097376</v>
       </c>
       <c r="O37" s="2">
-        <f>ABS(J37)+ABS(K37)+ABS(L37)+ABS(M37)</f>
+        <f t="shared" si="5"/>
         <v>0.93986320374069421</v>
       </c>
       <c r="P37" s="2">
-        <f>MIN(E37:I37)</f>
+        <f t="shared" si="6"/>
         <v>0.62699013948440496</v>
       </c>
       <c r="Q37" s="2">
-        <f>AVERAGE(E37:I37)</f>
+        <f t="shared" si="7"/>
         <v>0.64133883714675854</v>
       </c>
     </row>
@@ -3197,19 +3209,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N38" s="2">
-        <f>SUM(J38:M38)</f>
+        <f t="shared" si="4"/>
         <v>-6.843327447340157E-2</v>
       </c>
       <c r="O38" s="2">
-        <f>ABS(J38)+ABS(K38)+ABS(L38)+ABS(M38)</f>
+        <f t="shared" si="5"/>
         <v>0.50551065020003083</v>
       </c>
       <c r="P38" s="2">
-        <f>MIN(E38:I38)</f>
+        <f t="shared" si="6"/>
         <v>0.60981512069702104</v>
       </c>
       <c r="Q38" s="2">
-        <f>AVERAGE(E38:I38)</f>
+        <f t="shared" si="7"/>
         <v>0.64177572727203325</v>
       </c>
     </row>
@@ -3254,19 +3266,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N39" s="2">
-        <f>SUM(J39:M39)</f>
+        <f t="shared" si="4"/>
         <v>1.1452182958405017</v>
       </c>
       <c r="O39" s="2">
-        <f>ABS(J39)+ABS(K39)+ABS(L39)+ABS(M39)</f>
+        <f t="shared" si="5"/>
         <v>1.1452182958405017</v>
       </c>
       <c r="P39" s="2">
-        <f>MIN(E39:I39)</f>
+        <f t="shared" si="6"/>
         <v>0.61579287052154497</v>
       </c>
       <c r="Q39" s="2">
-        <f>AVERAGE(E39:I39)</f>
+        <f t="shared" si="7"/>
         <v>0.64177905321121165</v>
       </c>
     </row>
@@ -3311,19 +3323,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N40" s="2">
-        <f>SUM(J40:M40)</f>
+        <f t="shared" si="4"/>
         <v>0.11473890983692911</v>
       </c>
       <c r="O40" s="2">
-        <f>ABS(J40)+ABS(K40)+ABS(L40)+ABS(M40)</f>
+        <f t="shared" si="5"/>
         <v>0.36968428624725092</v>
       </c>
       <c r="P40" s="2">
-        <f>MIN(E40:I40)</f>
+        <f t="shared" si="6"/>
         <v>0.62564682960510198</v>
       </c>
       <c r="Q40" s="2">
-        <f>AVERAGE(E40:I40)</f>
+        <f t="shared" si="7"/>
         <v>0.64180438518524141</v>
       </c>
     </row>
@@ -3368,19 +3380,19 @@
         <v>0.20063232664151201</v>
       </c>
       <c r="N41" s="2">
-        <f>SUM(J41:M41)</f>
+        <f t="shared" si="4"/>
         <v>0.50940029631517303</v>
       </c>
       <c r="O41" s="2">
-        <f>ABS(J41)+ABS(K41)+ABS(L41)+ABS(M41)</f>
+        <f t="shared" si="5"/>
         <v>1.5932085857941989</v>
       </c>
       <c r="P41" s="2">
-        <f>MIN(E41:I41)</f>
+        <f t="shared" si="6"/>
         <v>0.631339251995086</v>
       </c>
       <c r="Q41" s="2">
-        <f>AVERAGE(E41:I41)</f>
+        <f t="shared" si="7"/>
         <v>0.64252645969390831</v>
       </c>
     </row>
@@ -3425,19 +3437,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N42" s="2">
-        <f>SUM(J42:M42)</f>
+        <f t="shared" si="4"/>
         <v>-0.49337661191180143</v>
       </c>
       <c r="O42" s="2">
-        <f>ABS(J42)+ABS(K42)+ABS(L42)+ABS(M42)</f>
+        <f t="shared" si="5"/>
         <v>0.8725797772252567</v>
       </c>
       <c r="P42" s="2">
-        <f>MIN(E42:I42)</f>
+        <f t="shared" si="6"/>
         <v>0.62735050916671697</v>
       </c>
       <c r="Q42" s="2">
-        <f>AVERAGE(E42:I42)</f>
+        <f t="shared" si="7"/>
         <v>0.6426656842231746</v>
       </c>
     </row>
@@ -3482,19 +3494,19 @@
         <v>4.2946836239538398E-2</v>
       </c>
       <c r="N43" s="2">
-        <f>SUM(J43:M43)</f>
+        <f t="shared" si="4"/>
         <v>0.3785130832233935</v>
       </c>
       <c r="O43" s="2">
-        <f>ABS(J43)+ABS(K43)+ABS(L43)+ABS(M43)</f>
+        <f t="shared" si="5"/>
         <v>1.0619117527934536</v>
       </c>
       <c r="P43" s="2">
-        <f>MIN(E43:I43)</f>
+        <f t="shared" si="6"/>
         <v>0.63252413272857599</v>
       </c>
       <c r="Q43" s="2">
-        <f>AVERAGE(E43:I43)</f>
+        <f t="shared" si="7"/>
         <v>0.64293367862701378</v>
       </c>
     </row>
@@ -3539,19 +3551,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N44" s="2">
-        <f>SUM(J44:M44)</f>
+        <f t="shared" si="4"/>
         <v>-7.1729120230275667E-2</v>
       </c>
       <c r="O44" s="2">
-        <f>ABS(J44)+ABS(K44)+ABS(L44)+ABS(M44)</f>
+        <f t="shared" si="5"/>
         <v>0.58027940050078808</v>
       </c>
       <c r="P44" s="2">
-        <f>MIN(E44:I44)</f>
+        <f t="shared" si="6"/>
         <v>0.60680276155471802</v>
       </c>
       <c r="Q44" s="2">
-        <f>AVERAGE(E44:I44)</f>
+        <f t="shared" si="7"/>
         <v>0.6431380510330198</v>
       </c>
     </row>
@@ -3596,19 +3608,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N45" s="2">
-        <f>SUM(J45:M45)</f>
+        <f t="shared" si="4"/>
         <v>6.0680276866183047E-2</v>
       </c>
       <c r="O45" s="2">
-        <f>ABS(J45)+ABS(K45)+ABS(L45)+ABS(M45)</f>
+        <f t="shared" si="5"/>
         <v>0.68033836756588306</v>
       </c>
       <c r="P45" s="2">
-        <f>MIN(E45:I45)</f>
+        <f t="shared" si="6"/>
         <v>0.63345110416412298</v>
       </c>
       <c r="Q45" s="2">
-        <f>AVERAGE(E45:I45)</f>
+        <f t="shared" si="7"/>
         <v>0.64320807456970186</v>
       </c>
     </row>
@@ -3653,19 +3665,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N46" s="2">
-        <f>SUM(J46:M46)</f>
+        <f t="shared" si="4"/>
         <v>-0.50101702905942691</v>
       </c>
       <c r="O46" s="2">
-        <f>ABS(J46)+ABS(K46)+ABS(L46)+ABS(M46)</f>
+        <f t="shared" si="5"/>
         <v>0.80915414651055917</v>
       </c>
       <c r="P46" s="2">
-        <f>MIN(E46:I46)</f>
+        <f t="shared" si="6"/>
         <v>0.63674604892730702</v>
       </c>
       <c r="Q46" s="2">
-        <f>AVERAGE(E46:I46)</f>
+        <f t="shared" si="7"/>
         <v>0.64329103231429996</v>
       </c>
     </row>
@@ -3710,19 +3722,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N47" s="2">
-        <f>SUM(J47:M47)</f>
+        <f t="shared" si="4"/>
         <v>-0.11427644459652038</v>
       </c>
       <c r="O47" s="2">
-        <f>ABS(J47)+ABS(K47)+ABS(L47)+ABS(M47)</f>
+        <f t="shared" si="5"/>
         <v>0.58660714574186767</v>
       </c>
       <c r="P47" s="2">
-        <f>MIN(E47:I47)</f>
+        <f t="shared" si="6"/>
         <v>0.62665730714797896</v>
       </c>
       <c r="Q47" s="2">
-        <f>AVERAGE(E47:I47)</f>
+        <f t="shared" si="7"/>
         <v>0.64378639459609954</v>
       </c>
     </row>
@@ -3767,19 +3779,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N48" s="2">
-        <f>SUM(J48:M48)</f>
+        <f t="shared" si="4"/>
         <v>0.72089591240917095</v>
       </c>
       <c r="O48" s="2">
-        <f>ABS(J48)+ABS(K48)+ABS(L48)+ABS(M48)</f>
+        <f t="shared" si="5"/>
         <v>2.0868523015462292</v>
       </c>
       <c r="P48" s="2">
-        <f>MIN(E48:I48)</f>
+        <f t="shared" si="6"/>
         <v>0.63330137729644698</v>
       </c>
       <c r="Q48" s="2">
-        <f>AVERAGE(E48:I48)</f>
+        <f t="shared" si="7"/>
         <v>0.64476909637451119</v>
       </c>
     </row>
@@ -3824,19 +3836,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N49" s="2">
-        <f>SUM(J49:M49)</f>
+        <f t="shared" si="4"/>
         <v>0.52960435163680875</v>
       </c>
       <c r="O49" s="2">
-        <f>ABS(J49)+ABS(K49)+ABS(L49)+ABS(M49)</f>
+        <f t="shared" si="5"/>
         <v>1.0596566139832626</v>
       </c>
       <c r="P49" s="2">
-        <f>MIN(E49:I49)</f>
+        <f t="shared" si="6"/>
         <v>0.62609136104583696</v>
       </c>
       <c r="Q49" s="2">
-        <f>AVERAGE(E49:I49)</f>
+        <f t="shared" si="7"/>
         <v>0.6451958656311032</v>
       </c>
     </row>
@@ -3881,19 +3893,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N50" s="2">
-        <f>SUM(J50:M50)</f>
+        <f t="shared" si="4"/>
         <v>0.91988492396531307</v>
       </c>
       <c r="O50" s="2">
-        <f>ABS(J50)+ABS(K50)+ABS(L50)+ABS(M50)</f>
+        <f t="shared" si="5"/>
         <v>1.052874041991025</v>
       </c>
       <c r="P50" s="2">
-        <f>MIN(E50:I50)</f>
+        <f t="shared" si="6"/>
         <v>0.62646877765655495</v>
       </c>
       <c r="Q50" s="2">
-        <f>AVERAGE(E50:I50)</f>
+        <f t="shared" si="7"/>
         <v>0.64555971622467001</v>
       </c>
     </row>
@@ -3938,19 +3950,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N51" s="2">
-        <f>SUM(J51:M51)</f>
+        <f t="shared" si="4"/>
         <v>0.51591890461899892</v>
       </c>
       <c r="O51" s="2">
-        <f>ABS(J51)+ABS(K51)+ABS(L51)+ABS(M51)</f>
+        <f t="shared" si="5"/>
         <v>0.9564964083743589</v>
       </c>
       <c r="P51" s="2">
-        <f>MIN(E51:I51)</f>
+        <f t="shared" si="6"/>
         <v>0.63441306352615301</v>
       </c>
       <c r="Q51" s="2">
-        <f>AVERAGE(E51:I51)</f>
+        <f t="shared" si="7"/>
         <v>0.64589903354644718</v>
       </c>
     </row>
@@ -3995,19 +4007,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N52" s="2">
-        <f>SUM(J52:M52)</f>
+        <f t="shared" si="4"/>
         <v>0.47059842595539109</v>
       </c>
       <c r="O52" s="2">
-        <f>ABS(J52)+ABS(K52)+ABS(L52)+ABS(M52)</f>
+        <f t="shared" si="5"/>
         <v>0.69696131204635114</v>
       </c>
       <c r="P52" s="2">
-        <f>MIN(E52:I52)</f>
+        <f t="shared" si="6"/>
         <v>0.63768351078033403</v>
       </c>
       <c r="Q52" s="2">
-        <f>AVERAGE(E52:I52)</f>
+        <f t="shared" si="7"/>
         <v>0.64684239625930728</v>
       </c>
     </row>
@@ -4052,19 +4064,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N53" s="2">
-        <f>SUM(J53:M53)</f>
+        <f t="shared" si="4"/>
         <v>0.4895485130097687</v>
       </c>
       <c r="O53" s="2">
-        <f>ABS(J53)+ABS(K53)+ABS(L53)+ABS(M53)</f>
+        <f t="shared" si="5"/>
         <v>0.4895485130097687</v>
       </c>
       <c r="P53" s="2">
-        <f>MIN(E53:I53)</f>
+        <f t="shared" si="6"/>
         <v>0.62046819925308205</v>
       </c>
       <c r="Q53" s="2">
-        <f>AVERAGE(E53:I53)</f>
+        <f t="shared" si="7"/>
         <v>0.64709074497222863</v>
       </c>
     </row>
@@ -4109,19 +4121,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N54" s="2">
-        <f>SUM(J54:M54)</f>
+        <f t="shared" si="4"/>
         <v>1.3834576552811819</v>
       </c>
       <c r="O54" s="2">
-        <f>ABS(J54)+ABS(K54)+ABS(L54)+ABS(M54)</f>
+        <f t="shared" si="5"/>
         <v>1.913509917627636</v>
       </c>
       <c r="P54" s="2">
-        <f>MIN(E54:I54)</f>
+        <f t="shared" si="6"/>
         <v>0.64066636562347401</v>
       </c>
       <c r="Q54" s="2">
-        <f>AVERAGE(E54:I54)</f>
+        <f t="shared" si="7"/>
         <v>0.64725105762481649</v>
       </c>
     </row>
@@ -4166,19 +4178,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N55" s="2">
-        <f>SUM(J55:M55)</f>
+        <f t="shared" si="4"/>
         <v>0.73244234587171297</v>
       </c>
       <c r="O55" s="2">
-        <f>ABS(J55)+ABS(K55)+ABS(L55)+ABS(M55)</f>
+        <f t="shared" si="5"/>
         <v>1.4158410154417731</v>
       </c>
       <c r="P55" s="2">
-        <f>MIN(E55:I55)</f>
+        <f t="shared" si="6"/>
         <v>0.62499058246612504</v>
       </c>
       <c r="Q55" s="2">
-        <f>AVERAGE(E55:I55)</f>
+        <f t="shared" si="7"/>
         <v>0.64754346609115543</v>
       </c>
     </row>
@@ -4223,19 +4235,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N56" s="2">
-        <f>SUM(J56:M56)</f>
+        <f t="shared" si="4"/>
         <v>0.92967120970920802</v>
       </c>
       <c r="O56" s="2">
-        <f>ABS(J56)+ABS(K56)+ABS(L56)+ABS(M56)</f>
+        <f t="shared" si="5"/>
         <v>1.322966414317948</v>
       </c>
       <c r="P56" s="2">
-        <f>MIN(E56:I56)</f>
+        <f t="shared" si="6"/>
         <v>0.635842025279998</v>
       </c>
       <c r="Q56" s="2">
-        <f>AVERAGE(E56:I56)</f>
+        <f t="shared" si="7"/>
         <v>0.64756660461425719</v>
       </c>
     </row>
@@ -4280,19 +4292,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N57" s="2">
-        <f>SUM(J57:M57)</f>
+        <f t="shared" si="4"/>
         <v>3.8397172835373472E-2</v>
       </c>
       <c r="O57" s="2">
-        <f>ABS(J57)+ABS(K57)+ABS(L57)+ABS(M57)</f>
+        <f t="shared" si="5"/>
         <v>0.79481232127278745</v>
       </c>
       <c r="P57" s="2">
-        <f>MIN(E57:I57)</f>
+        <f t="shared" si="6"/>
         <v>0.62718653678893999</v>
       </c>
       <c r="Q57" s="2">
-        <f>AVERAGE(E57:I57)</f>
+        <f t="shared" si="7"/>
         <v>0.64769631624221735</v>
       </c>
     </row>
@@ -4337,19 +4349,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N58" s="2">
-        <f>SUM(J58:M58)</f>
+        <f t="shared" si="4"/>
         <v>-0.32527191037227632</v>
       </c>
       <c r="O58" s="2">
-        <f>ABS(J58)+ABS(K58)+ABS(L58)+ABS(M58)</f>
+        <f t="shared" si="5"/>
         <v>0.75853637910674965</v>
       </c>
       <c r="P58" s="2">
-        <f>MIN(E58:I58)</f>
+        <f t="shared" si="6"/>
         <v>0.63104021549224798</v>
       </c>
       <c r="Q58" s="2">
-        <f>AVERAGE(E58:I58)</f>
+        <f t="shared" si="7"/>
         <v>0.64788860082626298</v>
       </c>
     </row>
@@ -4394,19 +4406,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N59" s="2">
-        <f>SUM(J59:M59)</f>
+        <f t="shared" si="4"/>
         <v>-3.4780803980530794E-2</v>
       </c>
       <c r="O59" s="2">
-        <f>ABS(J59)+ABS(K59)+ABS(L59)+ABS(M59)</f>
+        <f t="shared" si="5"/>
         <v>0.80285984409557121</v>
       </c>
       <c r="P59" s="2">
-        <f>MIN(E59:I59)</f>
+        <f t="shared" si="6"/>
         <v>0.63448733091354304</v>
       </c>
       <c r="Q59" s="2">
-        <f>AVERAGE(E59:I59)</f>
+        <f t="shared" si="7"/>
         <v>0.64813934564590403</v>
       </c>
     </row>
@@ -4451,19 +4463,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N60" s="2">
-        <f>SUM(J60:M60)</f>
+        <f t="shared" si="4"/>
         <v>6.1905848301133271E-2</v>
       </c>
       <c r="O60" s="2">
-        <f>ABS(J60)+ABS(K60)+ABS(L60)+ABS(M60)</f>
+        <f t="shared" si="5"/>
         <v>0.76278943863952131</v>
       </c>
       <c r="P60" s="2">
-        <f>MIN(E60:I60)</f>
+        <f t="shared" si="6"/>
         <v>0.63596999645233099</v>
       </c>
       <c r="Q60" s="2">
-        <f>AVERAGE(E60:I60)</f>
+        <f t="shared" si="7"/>
         <v>0.64826040267944285</v>
       </c>
     </row>
@@ -4508,19 +4520,19 @@
         <v>0.20063232664151201</v>
       </c>
       <c r="N61" s="2">
-        <f>SUM(J61:M61)</f>
+        <f t="shared" si="4"/>
         <v>0.85749877423558851</v>
       </c>
       <c r="O61" s="2">
-        <f>ABS(J61)+ABS(K61)+ABS(L61)+ABS(M61)</f>
+        <f t="shared" si="5"/>
         <v>0.99048789226130052</v>
       </c>
       <c r="P61" s="2">
-        <f>MIN(E61:I61)</f>
+        <f t="shared" si="6"/>
         <v>0.62857294082641602</v>
       </c>
       <c r="Q61" s="2">
-        <f>AVERAGE(E61:I61)</f>
+        <f t="shared" si="7"/>
         <v>0.64829878807067842</v>
       </c>
     </row>
@@ -4565,19 +4577,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N62" s="2">
-        <f>SUM(J62:M62)</f>
+        <f t="shared" si="4"/>
         <v>0.29311361861824903</v>
       </c>
       <c r="O62" s="2">
-        <f>ABS(J62)+ABS(K62)+ABS(L62)+ABS(M62)</f>
+        <f t="shared" si="5"/>
         <v>0.73369112237360901</v>
       </c>
       <c r="P62" s="2">
-        <f>MIN(E62:I62)</f>
+        <f t="shared" si="6"/>
         <v>0.63519686460494995</v>
       </c>
       <c r="Q62" s="2">
-        <f>AVERAGE(E62:I62)</f>
+        <f t="shared" si="7"/>
         <v>0.64848040342330893</v>
       </c>
     </row>
@@ -4622,19 +4634,19 @@
         <v>0.203822913829042</v>
       </c>
       <c r="N63" s="2">
-        <f>SUM(J63:M63)</f>
+        <f t="shared" si="4"/>
         <v>-0.1279519626842972</v>
       </c>
       <c r="O63" s="2">
-        <f>ABS(J63)+ABS(K63)+ABS(L63)+ABS(M63)</f>
+        <f t="shared" si="5"/>
         <v>0.5355977903423812</v>
       </c>
       <c r="P63" s="2">
-        <f>MIN(E63:I63)</f>
+        <f t="shared" si="6"/>
         <v>0.63507127761840798</v>
       </c>
       <c r="Q63" s="2">
-        <f>AVERAGE(E63:I63)</f>
+        <f t="shared" si="7"/>
         <v>0.64901067018508884</v>
       </c>
     </row>
@@ -4679,19 +4691,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N64" s="2">
-        <f>SUM(J64:M64)</f>
+        <f t="shared" si="4"/>
         <v>0.52847555246924038</v>
       </c>
       <c r="O64" s="2">
-        <f>ABS(J64)+ABS(K64)+ABS(L64)+ABS(M64)</f>
+        <f t="shared" si="5"/>
         <v>0.52847555246924038</v>
       </c>
       <c r="P64" s="2">
-        <f>MIN(E64:I64)</f>
+        <f t="shared" si="6"/>
         <v>0.63442265987396196</v>
       </c>
       <c r="Q64" s="2">
-        <f>AVERAGE(E64:I64)</f>
+        <f t="shared" si="7"/>
         <v>0.64918603897094684</v>
       </c>
     </row>
@@ -4736,19 +4748,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N65" s="2">
-        <f>SUM(J65:M65)</f>
+        <f t="shared" si="4"/>
         <v>-0.34475351361852602</v>
       </c>
       <c r="O65" s="2">
-        <f>ABS(J65)+ABS(K65)+ABS(L65)+ABS(M65)</f>
+        <f t="shared" si="5"/>
         <v>1.0650945378455106</v>
       </c>
       <c r="P65" s="2">
-        <f>MIN(E65:I65)</f>
+        <f t="shared" si="6"/>
         <v>0.63201647996902399</v>
       </c>
       <c r="Q65" s="2">
-        <f>AVERAGE(E65:I65)</f>
+        <f t="shared" si="7"/>
         <v>0.64918892383575399</v>
       </c>
     </row>
@@ -4793,19 +4805,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N66" s="2">
-        <f>SUM(J66:M66)</f>
+        <f t="shared" ref="N66:N97" si="8">SUM(J66:M66)</f>
         <v>1.0985953027374054</v>
       </c>
       <c r="O66" s="2">
-        <f>ABS(J66)+ABS(K66)+ABS(L66)+ABS(M66)</f>
+        <f t="shared" ref="O66:O97" si="9">ABS(J66)+ABS(K66)+ABS(L66)+ABS(M66)</f>
         <v>1.0985953027374054</v>
       </c>
       <c r="P66" s="2">
-        <f>MIN(E66:I66)</f>
+        <f t="shared" ref="P66:P97" si="10">MIN(E66:I66)</f>
         <v>0.63014721870422297</v>
       </c>
       <c r="Q66" s="2">
-        <f>AVERAGE(E66:I66)</f>
+        <f t="shared" ref="Q66:Q97" si="11">AVERAGE(E66:I66)</f>
         <v>0.64927773475646933</v>
       </c>
     </row>
@@ -4850,19 +4862,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N67" s="2">
-        <f>SUM(J67:M67)</f>
+        <f t="shared" si="8"/>
         <v>-9.2651068972266687E-2</v>
       </c>
       <c r="O67" s="2">
-        <f>ABS(J67)+ABS(K67)+ABS(L67)+ABS(M67)</f>
+        <f t="shared" si="9"/>
         <v>0.42260039402108307</v>
       </c>
       <c r="P67" s="2">
-        <f>MIN(E67:I67)</f>
+        <f t="shared" si="10"/>
         <v>0.63068282604217496</v>
       </c>
       <c r="Q67" s="2">
-        <f>AVERAGE(E67:I67)</f>
+        <f t="shared" si="11"/>
         <v>0.64984505176544138</v>
       </c>
     </row>
@@ -4907,19 +4919,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N68" s="2">
-        <f>SUM(J68:M68)</f>
+        <f t="shared" si="8"/>
         <v>0.69340371195614103</v>
       </c>
       <c r="O68" s="2">
-        <f>ABS(J68)+ABS(K68)+ABS(L68)+ABS(M68)</f>
+        <f t="shared" si="9"/>
         <v>0.91976659804710104</v>
       </c>
       <c r="P68" s="2">
-        <f>MIN(E68:I68)</f>
+        <f t="shared" si="10"/>
         <v>0.63230818510055498</v>
       </c>
       <c r="Q68" s="2">
-        <f>AVERAGE(E68:I68)</f>
+        <f t="shared" si="11"/>
         <v>0.64995774030685383</v>
       </c>
     </row>
@@ -4964,19 +4976,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N69" s="2">
-        <f>SUM(J69:M69)</f>
+        <f t="shared" si="8"/>
         <v>-8.7383361527779202E-2</v>
       </c>
       <c r="O69" s="2">
-        <f>ABS(J69)+ABS(K69)+ABS(L69)+ABS(M69)</f>
+        <f t="shared" si="9"/>
         <v>0.71292344923661322</v>
       </c>
       <c r="P69" s="2">
-        <f>MIN(E69:I69)</f>
+        <f t="shared" si="10"/>
         <v>0.63826161623001099</v>
       </c>
       <c r="Q69" s="2">
-        <f>AVERAGE(E69:I69)</f>
+        <f t="shared" si="11"/>
         <v>0.65149971246719318</v>
       </c>
     </row>
@@ -5021,19 +5033,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N70" s="2">
-        <f>SUM(J70:M70)</f>
+        <f t="shared" si="8"/>
         <v>0.95059315845119896</v>
       </c>
       <c r="O70" s="2">
-        <f>ABS(J70)+ABS(K70)+ABS(L70)+ABS(M70)</f>
+        <f t="shared" si="9"/>
         <v>1.4806454207976532</v>
       </c>
       <c r="P70" s="2">
-        <f>MIN(E70:I70)</f>
+        <f t="shared" si="10"/>
         <v>0.63152021169662398</v>
       </c>
       <c r="Q70" s="2">
-        <f>AVERAGE(E70:I70)</f>
+        <f t="shared" si="11"/>
         <v>0.65183470249175979</v>
       </c>
     </row>
@@ -5078,19 +5090,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N71" s="2">
-        <f>SUM(J71:M71)</f>
+        <f t="shared" si="8"/>
         <v>-0.49979145762447669</v>
       </c>
       <c r="O71" s="2">
-        <f>ABS(J71)+ABS(K71)+ABS(L71)+ABS(M71)</f>
+        <f t="shared" si="9"/>
         <v>0.89160521758419731</v>
       </c>
       <c r="P71" s="2">
-        <f>MIN(E71:I71)</f>
+        <f t="shared" si="10"/>
         <v>0.63735556602478005</v>
       </c>
       <c r="Q71" s="2">
-        <f>AVERAGE(E71:I71)</f>
+        <f t="shared" si="11"/>
         <v>0.65192509889602623</v>
       </c>
     </row>
@@ -5135,19 +5147,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N72" s="2">
-        <f>SUM(J72:M72)</f>
+        <f t="shared" si="8"/>
         <v>0.48702042713533011</v>
       </c>
       <c r="O72" s="2">
-        <f>ABS(J72)+ABS(K72)+ABS(L72)+ABS(M72)</f>
+        <f t="shared" si="9"/>
         <v>0.62000954516104212</v>
       </c>
       <c r="P72" s="2">
-        <f>MIN(E72:I72)</f>
+        <f t="shared" si="10"/>
         <v>0.64300376176834095</v>
       </c>
       <c r="Q72" s="2">
-        <f>AVERAGE(E72:I72)</f>
+        <f t="shared" si="11"/>
         <v>0.6523059964179988</v>
       </c>
     </row>
@@ -5192,19 +5204,19 @@
         <v>0.37126048128542699</v>
       </c>
       <c r="N73" s="2">
-        <f>SUM(J73:M73)</f>
+        <f t="shared" si="8"/>
         <v>-0.3057709376630553</v>
       </c>
       <c r="O73" s="2">
-        <f>ABS(J73)+ABS(K73)+ABS(L73)+ABS(M73)</f>
+        <f t="shared" si="9"/>
         <v>1.0482919002339093</v>
       </c>
       <c r="P73" s="2">
-        <f>MIN(E73:I73)</f>
+        <f t="shared" si="10"/>
         <v>0.63253009319305398</v>
       </c>
       <c r="Q73" s="2">
-        <f>AVERAGE(E73:I73)</f>
+        <f t="shared" si="11"/>
         <v>0.65361646413803043</v>
       </c>
     </row>
@@ -5249,19 +5261,19 @@
         <v>4.7400468259075297E-2</v>
       </c>
       <c r="N74" s="2">
-        <f>SUM(J74:M74)</f>
+        <f t="shared" si="8"/>
         <v>0.45782202888137136</v>
       </c>
       <c r="O74" s="2">
-        <f>ABS(J74)+ABS(K74)+ABS(L74)+ABS(M74)</f>
+        <f t="shared" si="9"/>
         <v>0.97307349187472114</v>
       </c>
       <c r="P74" s="2">
-        <f>MIN(E74:I74)</f>
+        <f t="shared" si="10"/>
         <v>0.62318170070648105</v>
       </c>
       <c r="Q74" s="2">
-        <f>AVERAGE(E74:I74)</f>
+        <f t="shared" si="11"/>
         <v>0.65363969802856414</v>
       </c>
     </row>
@@ -5306,19 +5318,19 @@
         <v>4.7400468259075297E-2</v>
       </c>
       <c r="N75" s="2">
-        <f>SUM(J75:M75)</f>
+        <f t="shared" si="8"/>
         <v>0.22520118748136175</v>
       </c>
       <c r="O75" s="2">
-        <f>ABS(J75)+ABS(K75)+ABS(L75)+ABS(M75)</f>
+        <f t="shared" si="9"/>
         <v>1.3090094769603879</v>
       </c>
       <c r="P75" s="2">
-        <f>MIN(E75:I75)</f>
+        <f t="shared" si="10"/>
         <v>0.631586253643035</v>
       </c>
       <c r="Q75" s="2">
-        <f>AVERAGE(E75:I75)</f>
+        <f t="shared" si="11"/>
         <v>0.65376327037811244</v>
       </c>
     </row>
@@ -5363,19 +5375,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N76" s="2">
-        <f>SUM(J76:M76)</f>
+        <f t="shared" si="8"/>
         <v>0.132040573672147</v>
       </c>
       <c r="O76" s="2">
-        <f>ABS(J76)+ABS(K76)+ABS(L76)+ABS(M76)</f>
+        <f t="shared" si="9"/>
         <v>0.57261807742750692</v>
       </c>
       <c r="P76" s="2">
-        <f>MIN(E76:I76)</f>
+        <f t="shared" si="10"/>
         <v>0.62691414356231601</v>
       </c>
       <c r="Q76" s="2">
-        <f>AVERAGE(E76:I76)</f>
+        <f t="shared" si="11"/>
         <v>0.6541556954383847</v>
       </c>
     </row>
@@ -5420,19 +5432,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N77" s="2">
-        <f>SUM(J77:M77)</f>
+        <f t="shared" si="8"/>
         <v>-0.13654858697131189</v>
       </c>
       <c r="O77" s="2">
-        <f>ABS(J77)+ABS(K77)+ABS(L77)+ABS(M77)</f>
+        <f t="shared" si="9"/>
         <v>0.77321296868970812</v>
       </c>
       <c r="P77" s="2">
-        <f>MIN(E77:I77)</f>
+        <f t="shared" si="10"/>
         <v>0.64305746555328303</v>
       </c>
       <c r="Q77" s="2">
-        <f>AVERAGE(E77:I77)</f>
+        <f t="shared" si="11"/>
         <v>0.65441163778305023</v>
       </c>
     </row>
@@ -5477,19 +5489,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N78" s="2">
-        <f>SUM(J78:M78)</f>
+        <f t="shared" si="8"/>
         <v>0.30952538100928906</v>
       </c>
       <c r="O78" s="2">
-        <f>ABS(J78)+ABS(K78)+ABS(L78)+ABS(M78)</f>
+        <f t="shared" si="9"/>
         <v>0.53588826710024917</v>
       </c>
       <c r="P78" s="2">
-        <f>MIN(E78:I78)</f>
+        <f t="shared" si="10"/>
         <v>0.63444268703460605</v>
       </c>
       <c r="Q78" s="2">
-        <f>AVERAGE(E78:I78)</f>
+        <f t="shared" si="11"/>
         <v>0.65480322837829519</v>
       </c>
     </row>
@@ -5534,19 +5546,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N79" s="2">
-        <f>SUM(J79:M79)</f>
+        <f t="shared" si="8"/>
         <v>-0.25316838011580678</v>
       </c>
       <c r="O79" s="2">
-        <f>ABS(J79)+ABS(K79)+ABS(L79)+ABS(M79)</f>
+        <f t="shared" si="9"/>
         <v>1.1382282950928673</v>
       </c>
       <c r="P79" s="2">
-        <f>MIN(E79:I79)</f>
+        <f t="shared" si="10"/>
         <v>0.63984167575836104</v>
       </c>
       <c r="Q79" s="2">
-        <f>AVERAGE(E79:I79)</f>
+        <f t="shared" si="11"/>
         <v>0.65485740900039624</v>
       </c>
     </row>
@@ -5591,19 +5603,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N80" s="2">
-        <f>SUM(J80:M80)</f>
+        <f t="shared" si="8"/>
         <v>1.1846108907575763</v>
       </c>
       <c r="O80" s="2">
-        <f>ABS(J80)+ABS(K80)+ABS(L80)+ABS(M80)</f>
+        <f t="shared" si="9"/>
         <v>1.1846108907575763</v>
       </c>
       <c r="P80" s="2">
-        <f>MIN(E80:I80)</f>
+        <f t="shared" si="10"/>
         <v>0.63047945499420099</v>
       </c>
       <c r="Q80" s="2">
-        <f>AVERAGE(E80:I80)</f>
+        <f t="shared" si="11"/>
         <v>0.65494902133941602</v>
       </c>
     </row>
@@ -5648,19 +5660,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N81" s="2">
-        <f>SUM(J81:M81)</f>
+        <f t="shared" si="8"/>
         <v>0.75927743447681406</v>
       </c>
       <c r="O81" s="2">
-        <f>ABS(J81)+ABS(K81)+ABS(L81)+ABS(M81)</f>
+        <f t="shared" si="9"/>
         <v>0.89226655250252618</v>
       </c>
       <c r="P81" s="2">
-        <f>MIN(E81:I81)</f>
+        <f t="shared" si="10"/>
         <v>0.63037979602813698</v>
       </c>
       <c r="Q81" s="2">
-        <f>AVERAGE(E81:I81)</f>
+        <f t="shared" si="11"/>
         <v>0.65512261390686011</v>
       </c>
     </row>
@@ -5705,19 +5717,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N82" s="2">
-        <f>SUM(J82:M82)</f>
+        <f t="shared" si="8"/>
         <v>0.54812220488376728</v>
       </c>
       <c r="O82" s="2">
-        <f>ABS(J82)+ABS(K82)+ABS(L82)+ABS(M82)</f>
+        <f t="shared" si="9"/>
         <v>0.54812220488376728</v>
       </c>
       <c r="P82" s="2">
-        <f>MIN(E82:I82)</f>
+        <f t="shared" si="10"/>
         <v>0.61897879838943404</v>
       </c>
       <c r="Q82" s="2">
-        <f>AVERAGE(E82:I82)</f>
+        <f t="shared" si="11"/>
         <v>0.6551448345184322</v>
       </c>
     </row>
@@ -5762,19 +5774,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N83" s="2">
-        <f>SUM(J83:M83)</f>
+        <f t="shared" si="8"/>
         <v>0.49809062640842094</v>
       </c>
       <c r="O83" s="2">
-        <f>ABS(J83)+ABS(K83)+ABS(L83)+ABS(M83)</f>
+        <f t="shared" si="9"/>
         <v>1.8640470155454791</v>
       </c>
       <c r="P83" s="2">
-        <f>MIN(E83:I83)</f>
+        <f t="shared" si="10"/>
         <v>0.63463306427001898</v>
       </c>
       <c r="Q83" s="2">
-        <f>AVERAGE(E83:I83)</f>
+        <f t="shared" si="11"/>
         <v>0.65532140731811461</v>
       </c>
     </row>
@@ -5819,19 +5831,19 @@
         <v>0.20063232664151201</v>
       </c>
       <c r="N84" s="2">
-        <f>SUM(J84:M84)</f>
+        <f t="shared" si="8"/>
         <v>-0.40279568930065257</v>
       </c>
       <c r="O84" s="2">
-        <f>ABS(J84)+ABS(K84)+ABS(L84)+ABS(M84)</f>
+        <f t="shared" si="9"/>
         <v>0.90737548626933351</v>
       </c>
       <c r="P84" s="2">
-        <f>MIN(E84:I84)</f>
+        <f t="shared" si="10"/>
         <v>0.61879301071166903</v>
       </c>
       <c r="Q84" s="2">
-        <f>AVERAGE(E84:I84)</f>
+        <f t="shared" si="11"/>
         <v>0.65551142692565867</v>
       </c>
     </row>
@@ -5876,19 +5888,19 @@
         <v>0.20063232664151201</v>
       </c>
       <c r="N85" s="2">
-        <f>SUM(J85:M85)</f>
+        <f t="shared" si="8"/>
         <v>-0.17017484790064288</v>
       </c>
       <c r="O85" s="2">
-        <f>ABS(J85)+ABS(K85)+ABS(L85)+ABS(M85)</f>
+        <f t="shared" si="9"/>
         <v>0.57143950118366693</v>
       </c>
       <c r="P85" s="2">
-        <f>MIN(E85:I85)</f>
+        <f t="shared" si="10"/>
         <v>0.63404279947280795</v>
       </c>
       <c r="Q85" s="2">
-        <f>AVERAGE(E85:I85)</f>
+        <f t="shared" si="11"/>
         <v>0.6558004975318904</v>
       </c>
     </row>
@@ -5933,19 +5945,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N86" s="2">
-        <f>SUM(J86:M86)</f>
+        <f t="shared" si="8"/>
         <v>-7.5349405137048797E-2</v>
       </c>
       <c r="O86" s="2">
-        <f>ABS(J86)+ABS(K86)+ABS(L86)+ABS(M86)</f>
+        <f t="shared" si="9"/>
         <v>0.62553418520133919</v>
       </c>
       <c r="P86" s="2">
-        <f>MIN(E86:I86)</f>
+        <f t="shared" si="10"/>
         <v>0.63417828083038297</v>
       </c>
       <c r="Q86" s="2">
-        <f>AVERAGE(E86:I86)</f>
+        <f t="shared" si="11"/>
         <v>0.65660597085952699</v>
       </c>
     </row>
@@ -5990,19 +6002,19 @@
         <v>0.36494717521125197</v>
       </c>
       <c r="N87" s="2">
-        <f>SUM(J87:M87)</f>
+        <f t="shared" si="8"/>
         <v>0.6657308059074224</v>
       </c>
       <c r="O87" s="2">
-        <f>ABS(J87)+ABS(K87)+ABS(L87)+ABS(M87)</f>
+        <f t="shared" si="9"/>
         <v>0.6657308059074224</v>
       </c>
       <c r="P87" s="2">
-        <f>MIN(E87:I87)</f>
+        <f t="shared" si="10"/>
         <v>0.63625609874725297</v>
       </c>
       <c r="Q87" s="2">
-        <f>AVERAGE(E87:I87)</f>
+        <f t="shared" si="11"/>
         <v>0.65663815736770559</v>
       </c>
     </row>
@@ -6047,19 +6059,19 @@
         <v>0.37126048128542699</v>
       </c>
       <c r="N88" s="2">
-        <f>SUM(J88:M88)</f>
+        <f t="shared" si="8"/>
         <v>1.3689310317455221</v>
       </c>
       <c r="O88" s="2">
-        <f>ABS(J88)+ABS(K88)+ABS(L88)+ABS(M88)</f>
+        <f t="shared" si="9"/>
         <v>2.0523297013155819</v>
       </c>
       <c r="P88" s="2">
-        <f>MIN(E88:I88)</f>
+        <f t="shared" si="10"/>
         <v>0.64284396171569802</v>
       </c>
       <c r="Q88" s="2">
-        <f>AVERAGE(E88:I88)</f>
+        <f t="shared" si="11"/>
         <v>0.65731053352355906</v>
       </c>
     </row>
@@ -6104,19 +6116,19 @@
         <v>0.37126048128542699</v>
       </c>
       <c r="N89" s="2">
-        <f>SUM(J89:M89)</f>
+        <f t="shared" si="8"/>
         <v>-0.1445984257373879</v>
       </c>
       <c r="O89" s="2">
-        <f>ABS(J89)+ABS(K89)+ABS(L89)+ABS(M89)</f>
+        <f t="shared" si="9"/>
         <v>0.88711938830824189</v>
       </c>
       <c r="P89" s="2">
-        <f>MIN(E89:I89)</f>
+        <f t="shared" si="10"/>
         <v>0.63495457172393799</v>
       </c>
       <c r="Q89" s="2">
-        <f>AVERAGE(E89:I89)</f>
+        <f t="shared" si="11"/>
         <v>0.65735915899276698</v>
       </c>
     </row>
@@ -6161,19 +6173,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N90" s="2">
-        <f>SUM(J90:M90)</f>
+        <f t="shared" si="8"/>
         <v>0.55188745566761832</v>
       </c>
       <c r="O90" s="2">
-        <f>ABS(J90)+ABS(K90)+ABS(L90)+ABS(M90)</f>
+        <f t="shared" si="9"/>
         <v>0.94518266027635833</v>
       </c>
       <c r="P90" s="2">
-        <f>MIN(E90:I90)</f>
+        <f t="shared" si="10"/>
         <v>0.63184291124343805</v>
       </c>
       <c r="Q90" s="2">
-        <f>AVERAGE(E90:I90)</f>
+        <f t="shared" si="11"/>
         <v>0.6581848382949822</v>
       </c>
     </row>
@@ -6218,19 +6230,19 @@
         <v>4.7400468259075297E-2</v>
       </c>
       <c r="N91" s="2">
-        <f>SUM(J91:M91)</f>
+        <f t="shared" si="8"/>
         <v>0.42906214008097776</v>
       </c>
       <c r="O91" s="2">
-        <f>ABS(J91)+ABS(K91)+ABS(L91)+ABS(M91)</f>
+        <f t="shared" si="9"/>
         <v>1.112460809651038</v>
       </c>
       <c r="P91" s="2">
-        <f>MIN(E91:I91)</f>
+        <f t="shared" si="10"/>
         <v>0.62780106067657404</v>
       </c>
       <c r="Q91" s="2">
-        <f>AVERAGE(E91:I91)</f>
+        <f t="shared" si="11"/>
         <v>0.65934201478958099</v>
       </c>
     </row>
@@ -6275,19 +6287,19 @@
         <v>4.7400468259075297E-2</v>
       </c>
       <c r="N92" s="2">
-        <f>SUM(J92:M92)</f>
+        <f t="shared" si="8"/>
         <v>0.50051046955532008</v>
       </c>
       <c r="O92" s="2">
-        <f>ABS(J92)+ABS(K92)+ABS(L92)+ABS(M92)</f>
+        <f t="shared" si="9"/>
         <v>0.93769733649103848</v>
       </c>
       <c r="P92" s="2">
-        <f>MIN(E92:I92)</f>
+        <f t="shared" si="10"/>
         <v>0.63969403505325295</v>
       </c>
       <c r="Q92" s="2">
-        <f>AVERAGE(E92:I92)</f>
+        <f t="shared" si="11"/>
         <v>0.65940295457839937</v>
       </c>
     </row>
@@ -6332,19 +6344,19 @@
         <v>0.20063232664151201</v>
       </c>
       <c r="N93" s="2">
-        <f>SUM(J93:M93)</f>
+        <f t="shared" si="8"/>
         <v>1.343354609582267</v>
       </c>
       <c r="O93" s="2">
-        <f>ABS(J93)+ABS(K93)+ABS(L93)+ABS(M93)</f>
+        <f t="shared" si="9"/>
         <v>1.7366498141910069</v>
       </c>
       <c r="P93" s="2">
-        <f>MIN(E93:I93)</f>
+        <f t="shared" si="10"/>
         <v>0.64699012041091897</v>
       </c>
       <c r="Q93" s="2">
-        <f>AVERAGE(E93:I93)</f>
+        <f t="shared" si="11"/>
         <v>0.6609976649284357</v>
       </c>
     </row>
@@ -6389,19 +6401,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N94" s="2">
-        <f>SUM(J94:M94)</f>
+        <f t="shared" si="8"/>
         <v>1.2228501657926831</v>
       </c>
       <c r="O94" s="2">
-        <f>ABS(J94)+ABS(K94)+ABS(L94)+ABS(M94)</f>
+        <f t="shared" si="9"/>
         <v>1.752902428139137</v>
       </c>
       <c r="P94" s="2">
-        <f>MIN(E94:I94)</f>
+        <f t="shared" si="10"/>
         <v>0.63750731945037797</v>
       </c>
       <c r="Q94" s="2">
-        <f>AVERAGE(E94:I94)</f>
+        <f t="shared" si="11"/>
         <v>0.6620430946350091</v>
       </c>
     </row>
@@ -6446,19 +6458,19 @@
         <v>7.1269476203103199E-2</v>
       </c>
       <c r="N95" s="2">
-        <f>SUM(J95:M95)</f>
+        <f t="shared" si="8"/>
         <v>-0.2820668575994757</v>
       </c>
       <c r="O95" s="2">
-        <f>ABS(J95)+ABS(K95)+ABS(L95)+ABS(M95)</f>
+        <f t="shared" si="9"/>
         <v>0.80174143187955027</v>
       </c>
       <c r="P95" s="2">
-        <f>MIN(E95:I95)</f>
+        <f t="shared" si="10"/>
         <v>0.64882904291152899</v>
       </c>
       <c r="Q95" s="2">
-        <f>AVERAGE(E95:I95)</f>
+        <f t="shared" si="11"/>
         <v>0.66212540864944414</v>
       </c>
     </row>
@@ -6503,19 +6515,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N96" s="2">
-        <f>SUM(J96:M96)</f>
+        <f t="shared" si="8"/>
         <v>0.36797390378359807</v>
       </c>
       <c r="O96" s="2">
-        <f>ABS(J96)+ABS(K96)+ABS(L96)+ABS(M96)</f>
+        <f t="shared" si="9"/>
         <v>1.451782193262624</v>
       </c>
       <c r="P96" s="2">
-        <f>MIN(E96:I96)</f>
+        <f t="shared" si="10"/>
         <v>0.65668791532516402</v>
       </c>
       <c r="Q96" s="2">
-        <f>AVERAGE(E96:I96)</f>
+        <f t="shared" si="11"/>
         <v>0.66427646875381419</v>
       </c>
     </row>
@@ -6560,19 +6572,19 @@
         <v>0.203822913829042</v>
       </c>
       <c r="N97" s="2">
-        <f>SUM(J97:M97)</f>
+        <f t="shared" si="8"/>
         <v>0.29838818758484981</v>
       </c>
       <c r="O97" s="2">
-        <f>ABS(J97)+ABS(K97)+ABS(L97)+ABS(M97)</f>
+        <f t="shared" si="9"/>
         <v>0.4752689679375402</v>
       </c>
       <c r="P97" s="2">
-        <f>MIN(E97:I97)</f>
+        <f t="shared" si="10"/>
         <v>0.63785094022750799</v>
       </c>
       <c r="Q97" s="2">
-        <f>AVERAGE(E97:I97)</f>
+        <f t="shared" si="11"/>
         <v>0.66488385200500455</v>
       </c>
     </row>
@@ -6617,19 +6629,19 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N98" s="2">
-        <f>SUM(J98:M98)</f>
+        <f t="shared" ref="N98:N129" si="12">SUM(J98:M98)</f>
         <v>-8.8700022433265399E-2</v>
       </c>
       <c r="O98" s="2">
-        <f>ABS(J98)+ABS(K98)+ABS(L98)+ABS(M98)</f>
+        <f t="shared" ref="O98:O107" si="13">ABS(J98)+ABS(K98)+ABS(L98)+ABS(M98)</f>
         <v>0.90228703286644263</v>
       </c>
       <c r="P98" s="2">
-        <f>MIN(E98:I98)</f>
+        <f t="shared" ref="P98:P107" si="14">MIN(E98:I98)</f>
         <v>0.61910808086395197</v>
       </c>
       <c r="Q98" s="2">
-        <f>AVERAGE(E98:I98)</f>
+        <f t="shared" ref="Q98:Q107" si="15">AVERAGE(E98:I98)</f>
         <v>0.66539951562881439</v>
       </c>
     </row>
@@ -6674,19 +6686,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N99" s="2">
-        <f>SUM(J99:M99)</f>
+        <f t="shared" si="12"/>
         <v>0.93798781324890634</v>
       </c>
       <c r="O99" s="2">
-        <f>ABS(J99)+ABS(K99)+ABS(L99)+ABS(M99)</f>
+        <f t="shared" si="13"/>
         <v>0.93798781324890634</v>
       </c>
       <c r="P99" s="2">
-        <f>MIN(E99:I99)</f>
+        <f t="shared" si="14"/>
         <v>0.645854532718658</v>
       </c>
       <c r="Q99" s="2">
-        <f>AVERAGE(E99:I99)</f>
+        <f t="shared" si="15"/>
         <v>0.66540400981902992</v>
       </c>
     </row>
@@ -6731,19 +6743,19 @@
         <v>0.14850641172078499</v>
       </c>
       <c r="N100" s="2">
-        <f>SUM(J100:M100)</f>
+        <f t="shared" si="12"/>
         <v>0.33701758146231897</v>
       </c>
       <c r="O100" s="2">
-        <f>ABS(J100)+ABS(K100)+ABS(L100)+ABS(M100)</f>
+        <f t="shared" si="13"/>
         <v>1.7029739705993772</v>
       </c>
       <c r="P100" s="2">
-        <f>MIN(E100:I100)</f>
+        <f t="shared" si="14"/>
         <v>0.64098548889160101</v>
       </c>
       <c r="Q100" s="2">
-        <f>AVERAGE(E100:I100)</f>
+        <f t="shared" si="15"/>
         <v>0.66714618206024112</v>
       </c>
     </row>
@@ -6788,19 +6800,19 @@
         <v>0.203822913829042</v>
       </c>
       <c r="N101" s="2">
-        <f>SUM(J101:M101)</f>
+        <f t="shared" si="12"/>
         <v>0.85703321877798544</v>
       </c>
       <c r="O101" s="2">
-        <f>ABS(J101)+ABS(K101)+ABS(L101)+ABS(M101)</f>
+        <f t="shared" si="13"/>
         <v>0.99002233680369756</v>
       </c>
       <c r="P101" s="2">
-        <f>MIN(E101:I101)</f>
+        <f t="shared" si="14"/>
         <v>0.63094979524612405</v>
       </c>
       <c r="Q101" s="2">
-        <f>AVERAGE(E101:I101)</f>
+        <f t="shared" si="15"/>
         <v>0.66743160486221287</v>
       </c>
     </row>
@@ -6845,19 +6857,19 @@
         <v>0.37126048128542699</v>
       </c>
       <c r="N102" s="2">
-        <f>SUM(J102:M102)</f>
+        <f t="shared" si="12"/>
         <v>1.1650700791459059</v>
       </c>
       <c r="O102" s="2">
-        <f>ABS(J102)+ABS(K102)+ABS(L102)+ABS(M102)</f>
+        <f t="shared" si="13"/>
         <v>2.2488783686249318</v>
       </c>
       <c r="P102" s="2">
-        <f>MIN(E102:I102)</f>
+        <f t="shared" si="14"/>
         <v>0.64855611324310303</v>
       </c>
       <c r="Q102" s="2">
-        <f>AVERAGE(E102:I102)</f>
+        <f t="shared" si="15"/>
         <v>0.66910864114761315</v>
       </c>
     </row>
@@ -6902,19 +6914,19 @@
         <v>0.37126048128542699</v>
       </c>
       <c r="N103" s="2">
-        <f>SUM(J103:M103)</f>
+        <f t="shared" si="12"/>
         <v>0.91183508519923706</v>
       </c>
       <c r="O103" s="2">
-        <f>ABS(J103)+ABS(K103)+ABS(L103)+ABS(M103)</f>
+        <f t="shared" si="13"/>
         <v>1.1667804616095587</v>
       </c>
       <c r="P103" s="2">
-        <f>MIN(E103:I103)</f>
+        <f t="shared" si="14"/>
         <v>0.64235973358154297</v>
       </c>
       <c r="Q103" s="2">
-        <f>AVERAGE(E103:I103)</f>
+        <f t="shared" si="15"/>
         <v>0.66973176002502399</v>
       </c>
     </row>
@@ -6959,19 +6971,19 @@
         <v>0.203822913829042</v>
       </c>
       <c r="N104" s="2">
-        <f>SUM(J104:M104)</f>
+        <f t="shared" si="12"/>
         <v>0.71279569345718596</v>
       </c>
       <c r="O104" s="2">
-        <f>ABS(J104)+ABS(K104)+ABS(L104)+ABS(M104)</f>
+        <f t="shared" si="13"/>
         <v>1.396194363027246</v>
       </c>
       <c r="P104" s="2">
-        <f>MIN(E104:I104)</f>
+        <f t="shared" si="14"/>
         <v>0.62797558307647705</v>
       </c>
       <c r="Q104" s="2">
-        <f>AVERAGE(E104:I104)</f>
+        <f t="shared" si="15"/>
         <v>0.6770449995994563</v>
       </c>
     </row>
@@ -7016,19 +7028,19 @@
         <v>0.203822913829042</v>
       </c>
       <c r="N105" s="2">
-        <f>SUM(J105:M105)</f>
+        <f t="shared" si="12"/>
         <v>1.3428890541246639</v>
       </c>
       <c r="O105" s="2">
-        <f>ABS(J105)+ABS(K105)+ABS(L105)+ABS(M105)</f>
+        <f t="shared" si="13"/>
         <v>1.7361842587334038</v>
       </c>
       <c r="P105" s="2">
-        <f>MIN(E105:I105)</f>
+        <f t="shared" si="14"/>
         <v>0.64327001571655196</v>
       </c>
       <c r="Q105" s="2">
-        <f>AVERAGE(E105:I105)</f>
+        <f t="shared" si="15"/>
         <v>0.67734137773513736</v>
       </c>
     </row>
@@ -7073,19 +7085,19 @@
         <v>0.31277004385441698</v>
       </c>
       <c r="N106" s="2">
-        <f>SUM(J106:M106)</f>
+        <f t="shared" si="12"/>
         <v>-0.13532301553636172</v>
       </c>
       <c r="O106" s="2">
-        <f>ABS(J106)+ABS(K106)+ABS(L106)+ABS(M106)</f>
+        <f t="shared" si="13"/>
         <v>0.85566403976334626</v>
       </c>
       <c r="P106" s="2">
-        <f>MIN(E106:I106)</f>
+        <f t="shared" si="14"/>
         <v>0.64215552806854204</v>
       </c>
       <c r="Q106" s="2">
-        <f>AVERAGE(E106:I106)</f>
+        <f t="shared" si="15"/>
         <v>0.67905930280685367</v>
       </c>
     </row>
@@ -7130,24 +7142,24 @@
         <v>3.5533023931161603E-2</v>
       </c>
       <c r="N107" s="2">
-        <f>SUM(J107:M107)</f>
+        <f t="shared" si="12"/>
         <v>-0.23478088838610439</v>
       </c>
       <c r="O107" s="2">
-        <f>ABS(J107)+ABS(K107)+ABS(L107)+ABS(M107)</f>
+        <f t="shared" si="13"/>
         <v>0.60285975968999761</v>
       </c>
       <c r="P107" s="2">
-        <f>MIN(E107:I107)</f>
+        <f t="shared" si="14"/>
         <v>0.65028762817382801</v>
       </c>
       <c r="Q107" s="2">
-        <f>AVERAGE(E107:I107)</f>
+        <f t="shared" si="15"/>
         <v>0.68278766870498608</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q107">
+  <autoFilter ref="A1:Q107" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q107">
       <sortCondition ref="Q1:Q107"/>
     </sortState>
@@ -7193,5 +7205,8 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="N2:Q107" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>